<commit_message>
Added metadata for Gronfier
</commit_message>
<xml_diff>
--- a/assets/translations/French.France.fr-FR.xlsx
+++ b/assets/translations/French.France.fr-FR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lbickerstaff/Nextcloud/PhD/Documents/Other/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mspitschan/Projects/LadenburgConsensusStatements/assets/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACC4C9E-925C-7440-9EF2-5550ED5C479C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBFEB50-8F61-7B49-95EA-230C20B4E55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13840" yWindow="-23520" windowWidth="38400" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="880" windowWidth="35080" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contributors" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="206">
   <si>
     <t>Number</t>
   </si>
@@ -670,12 +670,21 @@
   <si>
     <t>Principalement par le biais des ipRGCs, la lumière provoque la suppression de la mélatonine le soir et la nuit.</t>
   </si>
+  <si>
+    <t>claude.gronfier@inserm.fr</t>
+  </si>
+  <si>
+    <t>INSERM</t>
+  </si>
+  <si>
+    <t>0000-0002-6549-799X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -783,14 +792,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -986,7 +987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1055,7 +1056,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1065,7 +1065,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1452,8 +1452,18 @@
       <c r="B3" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="F3" s="11"/>
+      <c r="C3" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="4" spans="1:7" s="25" customFormat="1">
       <c r="A4" s="25" t="s">
@@ -1483,9 +1493,10 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{631FB3E8-CD59-A640-803C-2821653942A4}"/>
     <hyperlink ref="D4" r:id="rId2" xr:uid="{86F62BAB-6ED1-744B-94CA-1A037EE9E6BD}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{81C2DCD7-EB69-B941-826E-157D0F7C94BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1493,7 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1510,7 +1521,7 @@
       <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1539,10 +1550,10 @@
       <c r="A2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="26">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1568,8 +1579,8 @@
       <c r="A3" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="27">
+      <c r="B3" s="28"/>
+      <c r="C3" s="26">
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1595,8 +1606,8 @@
       <c r="A4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27">
+      <c r="B4" s="28"/>
+      <c r="C4" s="26">
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -1622,7 +1633,7 @@
       <c r="A5" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="7">
         <v>4</v>
       </c>
@@ -1649,7 +1660,7 @@
       <c r="A6" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="7">
         <v>5</v>
       </c>
@@ -1676,7 +1687,7 @@
       <c r="A7" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="7">
         <v>6</v>
       </c>
@@ -1703,7 +1714,7 @@
       <c r="A8" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>195</v>
       </c>
       <c r="C8" s="7">
@@ -1732,7 +1743,7 @@
       <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="7">
         <v>8</v>
       </c>
@@ -1759,7 +1770,7 @@
       <c r="A10" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="29"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="7">
         <v>9</v>
       </c>
@@ -1786,7 +1797,7 @@
       <c r="A11" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>196</v>
       </c>
       <c r="C11" s="7">
@@ -1815,7 +1826,7 @@
       <c r="A12" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="29"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="7">
         <v>11</v>
       </c>
@@ -1842,7 +1853,7 @@
       <c r="A13" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="7">
         <v>12</v>
       </c>
@@ -1869,7 +1880,7 @@
       <c r="A14" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="7">
         <v>13</v>
       </c>
@@ -1896,7 +1907,7 @@
       <c r="A15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="7">
         <v>14</v>
       </c>
@@ -1923,7 +1934,7 @@
       <c r="A16" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="7">
         <v>15</v>
       </c>
@@ -1950,7 +1961,7 @@
       <c r="A17" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="7">
         <v>16</v>
       </c>
@@ -1977,7 +1988,7 @@
       <c r="A18" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="7">
         <v>17</v>
       </c>
@@ -2004,7 +2015,7 @@
       <c r="A19" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="7">
         <v>18</v>
       </c>
@@ -2031,7 +2042,7 @@
       <c r="A20" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="7">
         <v>19</v>
       </c>
@@ -2058,7 +2069,7 @@
       <c r="A21" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="7">
         <v>20</v>
       </c>
@@ -2085,7 +2096,7 @@
       <c r="A22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>197</v>
       </c>
       <c r="C22" s="7">
@@ -2114,7 +2125,7 @@
       <c r="A23" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="29"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="7">
         <v>22</v>
       </c>
@@ -2141,7 +2152,7 @@
       <c r="A24" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="7">
         <v>23</v>
       </c>
@@ -2168,7 +2179,7 @@
       <c r="A25" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="28" t="s">
         <v>198</v>
       </c>
       <c r="C25" s="7">
@@ -2197,7 +2208,7 @@
       <c r="A26" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="7">
         <v>25</v>
       </c>
@@ -2224,7 +2235,7 @@
       <c r="A27" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="9">
         <v>26</v>
       </c>
@@ -2268,50 +2279,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="68">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="85">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="85">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="102">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>180</v>
       </c>
     </row>

</xml_diff>